<commit_message>
Switch example group numbers
</commit_message>
<xml_diff>
--- a/input/submitted_ratings/group_01/1.xlsx
+++ b/input/submitted_ratings/group_01/1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalia/Desktop/Seafile/2020 HS - HCI/Project/1 Instruction/Peer assessment/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chat/Seafile/2020 HS - HCI/Project/1 Instruction/Peer assessment/input/submitted_ratings/group_01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE5B4C7-06E2-A544-84D7-385F6A42F237}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3F7188-6E29-524B-8DB1-3C4EA4EC5721}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16160" windowHeight="15940" xr2:uid="{50EDE1AE-5C62-B246-8B6C-A7BCEBA9A8A5}"/>
+    <workbookView xWindow="9500" yWindow="980" windowWidth="16160" windowHeight="15940" xr2:uid="{50EDE1AE-5C62-B246-8B6C-A7BCEBA9A8A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>1: Made only a small contribution or contributed in a poor standard</t>
   </si>
@@ -83,13 +83,31 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Veselin</t>
+  </si>
+  <si>
+    <t>Rawda</t>
+  </si>
+  <si>
+    <t>Hannah</t>
+  </si>
+  <si>
+    <t>Mirit</t>
+  </si>
+  <si>
+    <t>Bogdana</t>
+  </si>
+  <si>
+    <t>Martin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,6 +119,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,9 +151,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DA1E63-6C45-C048-8516-400D26DBE315}">
-  <dimension ref="A2:E16"/>
+  <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,8 +530,8 @@
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -515,8 +541,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>11</v>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -526,8 +552,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>12</v>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -537,8 +563,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>13</v>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -548,13 +574,24 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>14</v>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="E17">
         <v>1</v>
       </c>
     </row>

</xml_diff>